<commit_message>
I have added two new files for create user.
</commit_message>
<xml_diff>
--- a/testdata/TestData.xlsx
+++ b/testdata/TestData.xlsx
@@ -1,20 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+  <workbookPr/>
+  <mc:AlternateContent>
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\neosoft\git\Title21Automation\testdata\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19380" windowHeight="6060"/>
+    <workbookView activeTab="3" firstSheet="1" windowHeight="8385" windowWidth="15405" xWindow="0" yWindow="2445"/>
   </bookViews>
   <sheets>
-    <sheet name="LoginCredentials" sheetId="1" r:id="rId1"/>
-    <sheet name="GroupDetails" sheetId="2" r:id="rId2"/>
-    <sheet name="CreateEmployee" sheetId="3" r:id="rId3"/>
+    <sheet name="LoginCredentials" r:id="rId1" sheetId="1"/>
+    <sheet name="GroupDetails" r:id="rId2" sheetId="2"/>
+    <sheet name="CreateEmployee" r:id="rId3" sheetId="3"/>
+    <sheet name="CreateUser" r:id="rId4" sheetId="5"/>
   </sheets>
-  <calcPr calcId="0"/>
-  <oleSize ref="A1:K18"/>
+  <calcPr calcId="0" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -22,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="42">
   <si>
     <t>sysadmin</t>
   </si>
@@ -111,16 +116,50 @@
     <t>martink@testmail.com</t>
   </si>
   <si>
-    <t>sameer</t>
-  </si>
-  <si>
-    <t>joshi12345</t>
+    <t>admin</t>
+  </si>
+  <si>
+    <t>administrator</t>
+  </si>
+  <si>
+    <t>Antioch</t>
+  </si>
+  <si>
+    <t>Bob</t>
+  </si>
+  <si>
+    <t>UserName</t>
+  </si>
+  <si>
+    <t>Bob123</t>
+  </si>
+  <si>
+    <t>AvailableFilter</t>
+  </si>
+  <si>
+    <t>QA</t>
+  </si>
+  <si>
+    <t>AuthenticationType</t>
+  </si>
+  <si>
+    <t>Title21</t>
+  </si>
+  <si>
+    <t>NewPassword</t>
+  </si>
+  <si>
+    <t>Bob@123456</t>
+  </si>
+  <si>
+    <t>ConfirmPassword</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="0"/>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -171,25 +210,26 @@
     </border>
   </borders>
   <cellStyleXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+  <cellXfs count="5">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="8" name="Hyperlink" xfId="1"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -206,10 +246,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -244,7 +284,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -279,7 +319,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -373,21 +413,21 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="6350">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="12700">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="19050">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -404,7 +444,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:outerShdw algn="ctr" blurRad="57150" dir="5400000" dist="19050" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="63000"/>
               </a:srgbClr>
@@ -456,33 +496,33 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" name="Office Theme" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.7109375" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="14.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="20.5703125" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="18.28515625" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="17.5703125" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="16.42578125" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="16.85546875" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="14.5703125" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="17" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="13.28515625" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="14.5703125" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="11.7109375" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="14.42578125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="20.5703125" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="18.28515625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="17.5703125" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="16.42578125" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="16.85546875" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="14.5703125" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="17.0" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="13.28515625" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="14.5703125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -523,13 +563,13 @@
       <c r="C5" s="1"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E9" sqref="E9"/>
@@ -554,36 +594,36 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:N4"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
+    <sheetView topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.85546875" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="14.42578125" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="16.7109375" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="14.5703125" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="16.28515625" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="13" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="22.42578125" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="18.42578125" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="14.42578125" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="17" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="13.140625" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="15.140625" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="23.140625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="13.85546875" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="14.42578125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="16.7109375" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="14.5703125" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="16.28515625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="13.0" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="22.0" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="18.42578125" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="14.42578125" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="17.0" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="13.140625" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="15.140625" collapsed="true"/>
+    <col min="13" max="13" customWidth="true" width="23.140625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="1" s="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>8</v>
       </c>
@@ -741,10 +781,75 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="M2" r:id="rId1"/>
-    <hyperlink ref="M3" r:id="rId2"/>
-    <hyperlink ref="M4" r:id="rId3"/>
+    <hyperlink r:id="rId1" ref="M2"/>
+    <hyperlink r:id="rId2" ref="M3"/>
+    <hyperlink r:id="rId3" ref="M4"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I17" sqref="I17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E1" t="s">
+        <v>37</v>
+      </c>
+      <c r="F1" t="s">
+        <v>39</v>
+      </c>
+      <c r="G1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D2" t="s">
+        <v>36</v>
+      </c>
+      <c r="E2" t="s">
+        <v>38</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>40</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink r:id="rId1" ref="F2"/>
+    <hyperlink r:id="rId2" ref="G2"/>
+  </hyperlinks>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated code for create user
</commit_message>
<xml_diff>
--- a/testdata/TestData.xlsx
+++ b/testdata/TestData.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView activeTab="3" firstSheet="1" windowHeight="8385" windowWidth="15405" xWindow="0" yWindow="2445"/>
+    <workbookView activeTab="3" windowHeight="8385" windowWidth="15405" xWindow="0" yWindow="2445"/>
   </bookViews>
   <sheets>
     <sheet name="LoginCredentials" r:id="rId1" sheetId="1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="41">
   <si>
     <t>sysadmin</t>
   </si>
@@ -122,24 +122,12 @@
     <t>administrator</t>
   </si>
   <si>
-    <t>Antioch</t>
-  </si>
-  <si>
-    <t>Bob</t>
-  </si>
-  <si>
     <t>UserName</t>
   </si>
   <si>
-    <t>Bob123</t>
-  </si>
-  <si>
     <t>AvailableFilter</t>
   </si>
   <si>
-    <t>QA</t>
-  </si>
-  <si>
     <t>AuthenticationType</t>
   </si>
   <si>
@@ -149,10 +137,19 @@
     <t>NewPassword</t>
   </si>
   <si>
-    <t>Bob@123456</t>
-  </si>
-  <si>
-    <t>ConfirmPassword</t>
+    <t>Martink401</t>
+  </si>
+  <si>
+    <t>Mart</t>
+  </si>
+  <si>
+    <t>mart123456</t>
+  </si>
+  <si>
+    <t>invalidePassword</t>
+  </si>
+  <si>
+    <t>mart12</t>
   </si>
 </sst>
 </file>
@@ -213,7 +210,7 @@
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
     <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyBorder="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
@@ -222,7 +219,6 @@
     <xf applyAlignment="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle builtinId="8" name="Hyperlink" xfId="1"/>
@@ -794,10 +790,19 @@
   <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I17" sqref="I17"/>
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" customWidth="true" width="14.42578125" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="16.0" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="16.42578125" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="15.85546875" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="14.140625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="17.5703125" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="16.0" collapsed="true"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -807,49 +812,49 @@
         <v>9</v>
       </c>
       <c r="C1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E1" t="s">
         <v>33</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
         <v>35</v>
       </c>
-      <c r="E1" t="s">
-        <v>37</v>
-      </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>39</v>
-      </c>
-      <c r="G1" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>31</v>
+        <v>6</v>
       </c>
       <c r="B2" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="C2" t="s">
+        <v>37</v>
+      </c>
+      <c r="D2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" t="s">
         <v>34</v>
       </c>
-      <c r="D2" t="s">
-        <v>36</v>
-      </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>38</v>
       </c>
-      <c r="F2" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="G2" s="4" t="s">
+      <c r="G2" t="s">
         <v>40</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink r:id="rId1" ref="F2"/>
-    <hyperlink r:id="rId2" ref="G2"/>
+    <hyperlink display="Bob@123456" r:id="rId1" ref="F2"/>
   </hyperlinks>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated files for 'create user' with negative and positive scenario
</commit_message>
<xml_diff>
--- a/testdata/TestData.xlsx
+++ b/testdata/TestData.xlsx
@@ -1,25 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\neosoft\git\Title21Automation\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView activeTab="1" windowHeight="6060" windowWidth="19380" xWindow="0" yWindow="0"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19380" windowHeight="6060" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="LoginCredentials" r:id="rId1" sheetId="1"/>
-    <sheet name="CreateUser" r:id="rId2" sheetId="4"/>
-    <sheet name="GroupDetails" r:id="rId3" sheetId="2"/>
-    <sheet name="CreateEmployee" r:id="rId4" sheetId="3"/>
+    <sheet name="LoginCredentials" sheetId="1" r:id="rId1"/>
+    <sheet name="CreateUser" sheetId="4" r:id="rId2"/>
+    <sheet name="GroupDetails" sheetId="2" r:id="rId3"/>
+    <sheet name="CreateEmployee" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="0" concurrentCalc="0"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="45">
   <si>
     <t>sysadmin</t>
   </si>
@@ -144,13 +144,30 @@
   </si>
   <si>
     <t>test123456</t>
+  </si>
+  <si>
+    <t>ShortPassword</t>
+  </si>
+  <si>
+    <t>test12</t>
+  </si>
+  <si>
+    <t>PasswordContaintUserName</t>
+  </si>
+  <si>
+    <t>Mart123456</t>
+  </si>
+  <si>
+    <t>WrongConfirmedPassword</t>
+  </si>
+  <si>
+    <t>test1234567</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="0"/>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -201,25 +218,25 @@
     </border>
   </borders>
   <cellStyleXfs count="2">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="4">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle builtinId="8" name="Hyperlink" xfId="1"/>
-    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -236,10 +253,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr lastClr="000000" val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr lastClr="FFFFFF" val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -274,7 +291,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin panose="020F0302020204030204" typeface="Calibri Light"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -309,7 +326,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin panose="020F0502020204030204" typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -403,21 +420,21 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="6350">
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="12700">
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="19050">
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -434,7 +451,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw algn="ctr" blurRad="57150" dir="5400000" dist="19050" rotWithShape="0">
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="63000"/>
               </a:srgbClr>
@@ -486,15 +503,15 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" name="Office Theme" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E10" sqref="E10"/>
@@ -502,17 +519,17 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="11.7109375" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="14.42578125" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="20.5703125" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="18.28515625" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="17.5703125" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="16.42578125" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="16.85546875" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="14.5703125" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" width="17.0" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" width="13.28515625" collapsed="true"/>
-    <col min="11" max="11" customWidth="true" width="14.5703125" collapsed="true"/>
+    <col min="1" max="1" width="11.7109375" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="14.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="20.5703125" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="18.28515625" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="17.5703125" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="16.42578125" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="16.85546875" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="14.5703125" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="17" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="13.28515625" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="14.5703125" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -553,29 +570,29 @@
       <c r="C5" s="1"/>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="8.42578125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="10.85546875" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="10.28515625" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="14.140625" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="18.85546875" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="13.7109375" collapsed="true"/>
+    <col min="1" max="1" width="8.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="10.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="10.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="18.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="13.7109375" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -594,8 +611,17 @@
       <c r="F1" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G1" t="s">
+        <v>39</v>
+      </c>
+      <c r="H1" t="s">
+        <v>41</v>
+      </c>
+      <c r="I1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -614,15 +640,24 @@
       <c r="F2" t="s">
         <v>38</v>
       </c>
+      <c r="G2" t="s">
+        <v>40</v>
+      </c>
+      <c r="H2" t="s">
+        <v>42</v>
+      </c>
+      <c r="I2" t="s">
+        <v>44</v>
+      </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E9" sqref="E9"/>
@@ -647,13 +682,13 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:M4"/>
   <sheetViews>
     <sheetView topLeftCell="C1" workbookViewId="0">
       <selection activeCell="J13" sqref="J13"/>
@@ -661,22 +696,22 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="13.85546875" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="14.42578125" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="16.7109375" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="14.5703125" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="16.28515625" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="13.0" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="22.42578125" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="18.42578125" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" width="14.42578125" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" width="17.0" collapsed="true"/>
-    <col min="11" max="11" customWidth="true" width="13.140625" collapsed="true"/>
-    <col min="12" max="12" customWidth="true" width="15.140625" collapsed="true"/>
-    <col min="13" max="13" customWidth="true" width="23.140625" collapsed="true"/>
+    <col min="1" max="1" width="13.85546875" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="14.42578125" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="16.7109375" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="14.5703125" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="16.28515625" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="13" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="22.42578125" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="18.42578125" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="14.42578125" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="17" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="13.140625" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="15.140625" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="23.140625" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row customFormat="1" r="1" s="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>8</v>
       </c>
@@ -834,10 +869,10 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink r:id="rId1" ref="M2"/>
-    <hyperlink r:id="rId2" ref="M3"/>
-    <hyperlink r:id="rId3" ref="M4"/>
+    <hyperlink ref="M2" r:id="rId1"/>
+    <hyperlink ref="M3" r:id="rId2"/>
+    <hyperlink ref="M4" r:id="rId3"/>
   </hyperlinks>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated files with two scenario for create new user
</commit_message>
<xml_diff>
--- a/testdata/TestData.xlsx
+++ b/testdata/TestData.xlsx
@@ -1,25 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\neosoft\git\Title21Automation\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19380" windowHeight="6060" activeTab="1"/>
+    <workbookView activeTab="1" windowHeight="6060" windowWidth="19380" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
-    <sheet name="LoginCredentials" sheetId="1" r:id="rId1"/>
-    <sheet name="CreateUser" sheetId="4" r:id="rId2"/>
-    <sheet name="GroupDetails" sheetId="2" r:id="rId3"/>
-    <sheet name="CreateEmployee" sheetId="3" r:id="rId4"/>
+    <sheet name="LoginCredentials" r:id="rId1" sheetId="1"/>
+    <sheet name="CreateUser" r:id="rId2" sheetId="4"/>
+    <sheet name="GroupDetails" r:id="rId3" sheetId="2"/>
+    <sheet name="CreateEmployee" r:id="rId4" sheetId="3"/>
   </sheets>
   <calcPr calcId="0" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -168,6 +168,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="0"/>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -218,25 +219,25 @@
     </border>
   </borders>
   <cellStyleXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="4">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="8" name="Hyperlink" xfId="1"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -253,10 +254,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -291,7 +292,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin panose="020F0302020204030204" typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -326,7 +327,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin panose="020F0502020204030204" typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -420,21 +421,21 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="6350">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="12700">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="19050">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -451,7 +452,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:outerShdw algn="ctr" blurRad="57150" dir="5400000" dist="19050" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="63000"/>
               </a:srgbClr>
@@ -503,15 +504,15 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" name="Office Theme" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E10" sqref="E10"/>
@@ -519,17 +520,17 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.7109375" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="14.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="20.5703125" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="18.28515625" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="17.5703125" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="16.42578125" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="16.85546875" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="14.5703125" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="17" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="13.28515625" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="14.5703125" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="11.7109375" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="14.42578125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="20.5703125" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="18.28515625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="17.5703125" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="16.42578125" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="16.85546875" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="14.5703125" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="17.0" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="13.28515625" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="14.5703125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -570,13 +571,13 @@
       <c r="C5" s="1"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="I11" sqref="I11"/>
@@ -584,12 +585,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="10.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="10.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="18.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="13.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="8.42578125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="10.85546875" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="10.28515625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="14.140625" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="18.85546875" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="13.7109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
@@ -651,13 +652,13 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E9" sqref="E9"/>
@@ -682,13 +683,13 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:N4"/>
   <sheetViews>
     <sheetView topLeftCell="C1" workbookViewId="0">
       <selection activeCell="J13" sqref="J13"/>
@@ -696,22 +697,22 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.85546875" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="14.42578125" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="16.7109375" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="14.5703125" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="16.28515625" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="13" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="22.42578125" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="18.42578125" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="14.42578125" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="17" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="13.140625" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="15.140625" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="23.140625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="13.85546875" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="14.42578125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="16.7109375" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="14.5703125" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="16.28515625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="13.0" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="22.42578125" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="18.42578125" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="14.42578125" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="17.0" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="13.140625" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="15.140625" collapsed="true"/>
+    <col min="13" max="13" customWidth="true" width="23.140625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="1" s="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>8</v>
       </c>
@@ -869,10 +870,10 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="M2" r:id="rId1"/>
-    <hyperlink ref="M3" r:id="rId2"/>
-    <hyperlink ref="M4" r:id="rId3"/>
+    <hyperlink r:id="rId1" ref="M2"/>
+    <hyperlink r:id="rId2" ref="M3"/>
+    <hyperlink r:id="rId3" ref="M4"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
committing changes on 22 Feb 2018
</commit_message>
<xml_diff>
--- a/testdata/TestData.xlsx
+++ b/testdata/TestData.xlsx
@@ -1,25 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\sameer\Title21Automation\testdata\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19380" windowHeight="6060" activeTab="3"/>
+    <workbookView activeTab="3" windowHeight="5970" windowWidth="19320" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
-    <sheet name="LoginCredentials" sheetId="1" r:id="rId1"/>
-    <sheet name="CreateUser" sheetId="4" r:id="rId2"/>
-    <sheet name="GroupDetails" sheetId="2" r:id="rId3"/>
-    <sheet name="CreateEmployee" sheetId="3" r:id="rId4"/>
+    <sheet name="LoginCredentials" r:id="rId1" sheetId="1"/>
+    <sheet name="CreateUser" r:id="rId2" sheetId="4"/>
+    <sheet name="GroupDetails" r:id="rId3" sheetId="2"/>
+    <sheet name="CreateEmployee" r:id="rId4" sheetId="3"/>
   </sheets>
   <calcPr calcId="0"/>
+  <oleSize ref="A1"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -152,13 +148,14 @@
     <t>Edit TX 75266-09023 edit Cross Lane</t>
   </si>
   <si>
-    <t xml:space="preserve"> Hetal P</t>
+    <t>john doe</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="0"/>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -209,25 +206,25 @@
     </border>
   </borders>
   <cellStyleXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="4">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="8" name="Hyperlink" xfId="1"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -244,10 +241,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -282,7 +279,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin panose="020F0302020204030204" typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -317,7 +314,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin panose="020F0502020204030204" typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -411,21 +408,21 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="6350">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="12700">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="19050">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -442,7 +439,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:outerShdw algn="ctr" blurRad="57150" dir="5400000" dist="19050" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="63000"/>
               </a:srgbClr>
@@ -494,15 +491,15 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" name="Office Theme" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E10" sqref="E10"/>
@@ -510,17 +507,17 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.7109375" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="14.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="20.5703125" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="18.28515625" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="17.5703125" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="16.42578125" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="16.85546875" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="14.5703125" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="17" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="13.28515625" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="14.5703125" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="11.7109375" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="14.42578125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="20.5703125" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="18.28515625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="17.5703125" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="16.42578125" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="16.85546875" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="14.5703125" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="17.0" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="13.28515625" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="14.5703125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -561,13 +558,13 @@
       <c r="C5" s="1"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F8" sqref="F8"/>
@@ -575,12 +572,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="10.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="10.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="18.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="13.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="8.42578125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="10.85546875" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="10.28515625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="14.140625" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="18.85546875" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="13.7109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -624,13 +621,13 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E9" sqref="E9"/>
@@ -655,36 +652,36 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:N4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.85546875" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="14.42578125" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="16.7109375" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="14.5703125" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="16.28515625" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="13" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="24.5703125" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="18.42578125" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="14.42578125" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="17" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="13.140625" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="15.140625" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="23.140625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="13.85546875" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="14.42578125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="16.7109375" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="14.5703125" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="16.28515625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="16.5703125" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="38.0" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="14.7109375" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="15.7109375" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="17.0" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="13.140625" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="15.140625" collapsed="true"/>
+    <col min="13" max="13" customWidth="true" width="23.140625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="1" s="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>8</v>
       </c>
@@ -820,9 +817,9 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="M2" r:id="rId1"/>
-    <hyperlink ref="M3" r:id="rId2"/>
+    <hyperlink r:id="rId1" ref="M2"/>
+    <hyperlink r:id="rId2" ref="M3"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
changes - add link to test case document.
</commit_message>
<xml_diff>
--- a/testdata/TestData.xlsx
+++ b/testdata/TestData.xlsx
@@ -3,13 +3,8 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent>
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\neosoft\git\Title21Automation\testdata\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView activeTab="1" windowHeight="6060" windowWidth="19380" xWindow="0" yWindow="0"/>
+    <workbookView activeTab="3" windowHeight="5970" windowWidth="16980" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
     <sheet name="LoginCredentials" r:id="rId1" sheetId="1"/>
@@ -18,6 +13,7 @@
     <sheet name="CreateEmployee" r:id="rId4" sheetId="3"/>
   </sheets>
   <calcPr calcId="0" concurrentCalc="0"/>
+  <oleSize ref="C1:L17"/>
   <extLst>
     <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -92,9 +88,6 @@
     <t>email</t>
   </si>
   <si>
-    <t>Martink</t>
-  </si>
-  <si>
     <t>Hetal M</t>
   </si>
   <si>
@@ -162,6 +155,9 @@
   </si>
   <si>
     <t>test1234567</t>
+  </si>
+  <si>
+    <t>AdamG</t>
   </si>
 </sst>
 </file>
@@ -546,10 +542,10 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>29</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>30</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>3</v>
@@ -579,18 +575,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" bestFit="true" customWidth="true" width="8.42578125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="10.85546875" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="12.0" collapsed="true"/>
     <col min="3" max="3" bestFit="true" customWidth="true" width="10.28515625" collapsed="true"/>
     <col min="4" max="4" bestFit="true" customWidth="true" width="14.140625" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="18.85546875" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="13.7109375" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="19.140625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="15.85546875" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="15.5703125" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="15.0" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="15.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
@@ -601,25 +600,25 @@
         <v>9</v>
       </c>
       <c r="C1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D1" t="s">
         <v>31</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>32</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>33</v>
       </c>
-      <c r="F1" t="s">
-        <v>34</v>
-      </c>
       <c r="G1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="I1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -627,28 +626,28 @@
         <v>6</v>
       </c>
       <c r="B2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C2" t="s">
         <v>35</v>
-      </c>
-      <c r="C2" t="s">
-        <v>36</v>
       </c>
       <c r="D2" t="s">
         <v>6</v>
       </c>
       <c r="E2" t="s">
+        <v>36</v>
+      </c>
+      <c r="F2" t="s">
         <v>37</v>
       </c>
-      <c r="F2" t="s">
-        <v>38</v>
-      </c>
       <c r="G2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="I2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
   </sheetData>
@@ -691,8 +690,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N4"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -758,75 +757,75 @@
         <v>6</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C2" s="2">
+        <v>1540</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>21</v>
-      </c>
-      <c r="C2" s="2">
-        <v>1267</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>22</v>
       </c>
       <c r="E2" s="2"/>
       <c r="F2" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G2" s="2" t="s">
         <v>23</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>24</v>
       </c>
       <c r="H2" s="2" t="s">
         <v>6</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="J2" s="2">
         <v>660675</v>
       </c>
       <c r="K2" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="L2" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="L2" s="2" t="s">
+      <c r="M2" s="3" t="s">
         <v>27</v>
-      </c>
-      <c r="M2" s="3" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="2"/>
       <c r="B3" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C3" s="2">
+        <v>1540</v>
+      </c>
+      <c r="D3" s="2" t="s">
         <v>21</v>
-      </c>
-      <c r="C3" s="2">
-        <v>1267</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>22</v>
       </c>
       <c r="E3" s="2"/>
       <c r="F3" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G3" s="2" t="s">
         <v>23</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>24</v>
       </c>
       <c r="H3" s="2" t="s">
         <v>6</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="J3" s="2">
         <v>660675</v>
       </c>
       <c r="K3" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="L3" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="L3" s="2" t="s">
+      <c r="M3" s="3" t="s">
         <v>27</v>
-      </c>
-      <c r="M3" s="3" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
@@ -834,38 +833,38 @@
         <v>6</v>
       </c>
       <c r="B4" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C4" s="2">
+        <v>1540</v>
+      </c>
+      <c r="D4" s="2" t="s">
         <v>21</v>
-      </c>
-      <c r="C4" s="2">
-        <v>1267</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>22</v>
       </c>
       <c r="E4" s="2"/>
       <c r="F4" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G4" s="2" t="s">
         <v>23</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>24</v>
       </c>
       <c r="H4" s="2" t="s">
         <v>6</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="J4" s="2">
         <v>660675</v>
       </c>
       <c r="K4" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="L4" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="L4" s="2" t="s">
+      <c r="M4" s="3" t="s">
         <v>27</v>
-      </c>
-      <c r="M4" s="3" t="s">
-        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added Account Lockout Test in Test package
</commit_message>
<xml_diff>
--- a/testdata/TestData.xlsx
+++ b/testdata/TestData.xlsx
@@ -4,20 +4,20 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowHeight="10320" windowWidth="23420"/>
+    <workbookView windowWidth="23420" windowHeight="10320"/>
   </bookViews>
   <sheets>
-    <sheet name="LoginCredentials" r:id="rId1" sheetId="1"/>
-    <sheet name="CreateUser" r:id="rId2" sheetId="2"/>
-    <sheet name="GroupDetails" r:id="rId3" sheetId="3"/>
-    <sheet name="CreateEmployee" r:id="rId4" sheetId="4"/>
+    <sheet name="LoginCredentials" sheetId="1" r:id="rId1"/>
+    <sheet name="CreateUser" sheetId="2" r:id="rId2"/>
+    <sheet name="GroupDetails" sheetId="3" r:id="rId3"/>
+    <sheet name="CreateEmployee" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="144525" concurrentCalc="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="0">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49">
   <si>
     <t>Admin</t>
   </si>
@@ -46,7 +46,7 @@
     <t>testlock123</t>
   </si>
   <si>
-    <t>Account Lock Out Test</t>
+    <t>Account Lockout Test</t>
   </si>
   <si>
     <t>Location</t>
@@ -171,8 +171,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
@@ -226,49 +226,49 @@
     </border>
   </borders>
   <cellStyleXfs count="7">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="0" numFmtId="176">
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="0" numFmtId="44">
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="0" numFmtId="177">
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="0" numFmtId="9">
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="0" numFmtId="42">
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="1" numFmtId="0">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
   <cellXfs count="5">
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="6">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="6" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" applyBorder="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="7">
-    <cellStyle builtinId="0" name="Normal" xfId="0"/>
-    <cellStyle builtinId="3" name="Comma" xfId="1"/>
-    <cellStyle builtinId="4" name="Currency" xfId="2"/>
-    <cellStyle builtinId="6" name="Comma[0]" xfId="3"/>
-    <cellStyle builtinId="5" name="Percent" xfId="4"/>
-    <cellStyle builtinId="7" name="Currency[0]" xfId="5"/>
-    <cellStyle builtinId="8" name="Hyperlink" xfId="6"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Comma" xfId="1" builtinId="3"/>
+    <cellStyle name="Currency" xfId="2" builtinId="4"/>
+    <cellStyle name="Comma[0]" xfId="3" builtinId="6"/>
+    <cellStyle name="Percent" xfId="4" builtinId="5"/>
+    <cellStyle name="Currency[0]" xfId="5" builtinId="7"/>
+    <cellStyle name="Hyperlink" xfId="6" builtinId="8"/>
   </cellStyles>
 </styleSheet>
 </file>
@@ -278,10 +278,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr lastClr="000000" val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr lastClr="FFFFFF" val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -439,7 +439,7 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="9525">
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="95000"/>
@@ -448,13 +448,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="25400">
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="38100">
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -464,7 +464,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dir="5400000" dist="20000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -473,7 +473,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dir="5400000" dist="23000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -482,7 +482,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dir="5400000" dist="23000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -492,12 +492,12 @@
             <a:camera prst="orthographicFront">
               <a:rot lat="0" lon="0" rev="0"/>
             </a:camera>
-            <a:lightRig dir="t" rig="threePt">
+            <a:lightRig rig="threePt" dir="t">
               <a:rot lat="0" lon="0" rev="1200000"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
-            <a:bevelT h="25400" w="63500"/>
+            <a:bevelT w="63500" h="25400"/>
           </a:sp3d>
         </a:effectStyle>
       </a:effectStyleLst>
@@ -528,7 +528,7 @@
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect b="180000" l="50000" r="50000" t="-80000"/>
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
           </a:path>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
@@ -547,7 +547,7 @@
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect b="50000" l="50000" r="50000" t="50000"/>
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
           </a:path>
         </a:gradFill>
       </a:bgFillStyleLst>
@@ -563,13 +563,13 @@
         <a:custGeom>
           <a:avLst/>
           <a:gdLst>
-            <a:gd fmla="val 21600" name="_h"/>
-            <a:gd fmla="val 21600" name="_w"/>
+            <a:gd name="_h" fmla="val 21600"/>
+            <a:gd name="_w" fmla="val 21600"/>
           </a:gdLst>
           <a:ahLst/>
           <a:cxnLst/>
           <a:pathLst>
-            <a:path h="21600" w="21600"/>
+            <a:path w="21600" h="21600"/>
           </a:pathLst>
         </a:custGeom>
         <a:gradFill rotWithShape="0">
@@ -583,7 +583,7 @@
           </a:gsLst>
           <a:lin ang="5400000" scaled="0"/>
         </a:gradFill>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="15875">
+        <a:ln w="15875" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:srgbClr val="739CC3"/>
           </a:solidFill>
@@ -600,27 +600,27 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelCol="3" outlineLevelRow="4"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelRow="4" outlineLevelCol="3"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="11.7142857142857" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="14.4285714285714" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="20.5714285714286" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="22.1428571428571" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="17.5714285714286" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="16.4285714285714" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="16.8571428571429" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="14.5714285714286" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" width="17.0" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" width="13.2857142857143" collapsed="true"/>
-    <col min="11" max="11" customWidth="true" width="14.5714285714286" collapsed="true"/>
+    <col min="1" max="1" width="11.7142857142857" customWidth="1"/>
+    <col min="2" max="2" width="14.4285714285714" customWidth="1"/>
+    <col min="3" max="3" width="20.5714285714286" customWidth="1"/>
+    <col min="4" max="4" width="22.1428571428571" customWidth="1"/>
+    <col min="5" max="5" width="17.5714285714286" customWidth="1"/>
+    <col min="6" max="6" width="16.4285714285714" customWidth="1"/>
+    <col min="7" max="7" width="16.8571428571429" customWidth="1"/>
+    <col min="8" max="8" width="14.5714285714286" customWidth="1"/>
+    <col min="9" max="9" width="17" customWidth="1"/>
+    <col min="10" max="10" width="13.2857142857143" customWidth="1"/>
+    <col min="11" max="11" width="14.5714285714286" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -670,16 +670,16 @@
       <c r="C5" s="3"/>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.699305555555556" right="0.699305555555556" top="0.75"/>
-  <pageSetup orientation="portrait" paperSize="9"/>
+  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
-  <dimension ref="A1:J2"/>
+  <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="I11" sqref="I11"/>
@@ -687,12 +687,12 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelRow="1"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="8.42857142857143" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="10.8571428571429" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="10.2857142857143" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="14.1428571428571" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="18.8571428571429" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="13.7142857142857" collapsed="true"/>
+    <col min="1" max="1" width="8.42857142857143" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="10.8571428571429" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="10.2857142857143" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="14.1428571428571" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="18.8571428571429" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="13.7142857142857" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
@@ -754,22 +754,22 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.699305555555556" right="0.699305555555556" top="0.75"/>
-  <pageSetup orientation="portrait" paperSize="9"/>
+  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelCol="1" outlineLevelRow="1"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelRow="1" outlineLevelCol="1"/>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
@@ -788,16 +788,16 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.699305555555556" right="0.699305555555556" top="0.75"/>
-  <pageSetup orientation="portrait" paperSize="9"/>
+  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
-  <dimension ref="A1:N4"/>
+  <dimension ref="A1:M4"/>
   <sheetViews>
     <sheetView topLeftCell="C1" workbookViewId="0">
       <selection activeCell="J13" sqref="J13"/>
@@ -805,22 +805,22 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelRow="3"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="13.8571428571429" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="14.4285714285714" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="16.7142857142857" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="14.5714285714286" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="16.2857142857143" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="13.0" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="22.4285714285714" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="18.4285714285714" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" width="14.4285714285714" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" width="17.0" collapsed="true"/>
-    <col min="11" max="11" customWidth="true" width="13.1428571428571" collapsed="true"/>
-    <col min="12" max="12" customWidth="true" width="15.1428571428571" collapsed="true"/>
-    <col min="13" max="13" customWidth="true" width="23.1428571428571" collapsed="true"/>
+    <col min="1" max="1" width="13.8571428571429" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="14.4285714285714" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="16.7142857142857" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="14.5714285714286" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="16.2857142857143" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="13" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="22.4285714285714" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="18.4285714285714" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="14.4285714285714" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="17" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="13.1428571428571" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="15.1428571428571" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="23.1428571428571" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row customFormat="1" r="1" s="1" spans="1:13">
+    <row r="1" s="1" customFormat="1" spans="1:13">
       <c r="A1" s="1" t="s">
         <v>29</v>
       </c>
@@ -978,12 +978,12 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink display="martink@testmail.com" r:id="rId1" ref="M4"/>
-    <hyperlink display="martink@testmail.com" r:id="rId1" ref="M3"/>
-    <hyperlink display="martink@testmail.com" r:id="rId1" ref="M2"/>
+    <hyperlink ref="M4" r:id="rId1" display="martink@testmail.com"/>
+    <hyperlink ref="M3" r:id="rId1" display="martink@testmail.com"/>
+    <hyperlink ref="M2" r:id="rId1" display="martink@testmail.com"/>
   </hyperlinks>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.699305555555556" right="0.699305555555556" top="0.75"/>
-  <pageSetup orientation="portrait" paperSize="9"/>
+  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>
 </file>
</xml_diff>